<commit_message>
Process rapport + Tidsplan
</commit_message>
<xml_diff>
--- a/Bachelor Rapport/Projektplan.xlsx
+++ b/Bachelor Rapport/Projektplan.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m_s_k\Documents\IKT\7.Semester\Bachelor-Rapport\Forprojekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m_s_k\Documents\IKT\7.Semester\Bachelor-TilsynRamboell-\Bachelor Rapport\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Juli</t>
   </si>
@@ -60,12 +60,33 @@
   </si>
   <si>
     <t>Final test med Rambøll</t>
+  </si>
+  <si>
+    <t>Rapport og dokumentation</t>
+  </si>
+  <si>
+    <t>Produkt</t>
+  </si>
+  <si>
+    <t>Kravspecifikation dokumentation og rapport done</t>
+  </si>
+  <si>
+    <t>Arkitektur og projekt beskrivelse dokumentation og rapport done</t>
+  </si>
+  <si>
+    <t>Sidste korrektur læsning</t>
+  </si>
+  <si>
+    <t>Design dokumentation og rapport done</t>
+  </si>
+  <si>
+    <t>Process rapporten: Gruppedannelse, Samarbejdsaftale og Projektledelse done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -83,7 +104,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -138,7 +159,31 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom style="medium">
@@ -147,7 +192,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
@@ -162,24 +207,65 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -189,21 +275,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -211,28 +288,23 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -243,6 +315,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -252,22 +368,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,379 +699,514 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:M16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="13" max="13" width="16" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+    </row>
+    <row r="3" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="4" t="s">
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="13"/>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="26"/>
+    </row>
+    <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="1">
         <v>27</v>
       </c>
-      <c r="B4" s="2">
+      <c r="D4" s="2">
         <v>28</v>
       </c>
-      <c r="C4" s="2">
+      <c r="E4" s="2">
         <v>29</v>
       </c>
-      <c r="D4" s="3">
+      <c r="F4" s="3">
         <v>30</v>
       </c>
-      <c r="E4" s="1">
+      <c r="G4" s="1">
         <v>31</v>
       </c>
-      <c r="F4" s="2">
+      <c r="H4" s="2">
         <v>32</v>
       </c>
-      <c r="G4" s="2">
+      <c r="I4" s="2">
         <v>33</v>
       </c>
-      <c r="H4" s="3">
+      <c r="J4" s="3">
         <v>34</v>
       </c>
-      <c r="I4" s="1">
+      <c r="K4" s="1">
         <v>35</v>
       </c>
-      <c r="J4" s="2">
+      <c r="L4" s="2">
         <v>36</v>
       </c>
-      <c r="K4" s="2">
+      <c r="M4" s="2">
         <v>37</v>
       </c>
-      <c r="L4" s="2">
+      <c r="N4" s="2">
         <v>38</v>
       </c>
-      <c r="M4" s="2">
+      <c r="O4" s="3">
         <v>39</v>
       </c>
-      <c r="N4" s="17"/>
-      <c r="O4" s="18"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="10" t="s">
+    </row>
+    <row r="5" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="H5" s="9"/>
+      <c r="I5" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="10" t="s">
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="8"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="18"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="O5" s="11"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="28"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="18"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="12"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="28"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="18"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="12"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="28"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="18"/>
-    </row>
-    <row r="9" spans="1:15" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="18"/>
-    </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="G8" s="22"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="12"/>
+    </row>
+    <row r="9" spans="2:18" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="29"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="16"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="N10" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="O10" s="11"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="31"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="12"/>
+    </row>
+    <row r="12" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="31"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="12"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="31"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="12"/>
+    </row>
+    <row r="14" spans="2:18" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="32"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="16"/>
+    </row>
+    <row r="15" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="4" t="s">
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="4" t="s">
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="18"/>
-    </row>
-    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="26"/>
+    </row>
+    <row r="16" spans="2:18" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="1">
         <v>40</v>
       </c>
-      <c r="B11" s="2">
+      <c r="D16" s="2">
         <v>41</v>
       </c>
-      <c r="C11" s="2">
+      <c r="E16" s="2">
         <v>42</v>
       </c>
-      <c r="D11" s="3">
+      <c r="F16" s="3">
         <v>43</v>
       </c>
-      <c r="E11" s="1">
+      <c r="G16" s="1">
         <v>44</v>
       </c>
-      <c r="F11" s="2">
+      <c r="H16" s="2">
         <v>45</v>
       </c>
-      <c r="G11" s="2">
+      <c r="I16" s="2">
         <v>46</v>
       </c>
-      <c r="H11" s="2">
+      <c r="J16" s="2">
         <v>47</v>
       </c>
-      <c r="I11" s="3">
+      <c r="K16" s="3">
         <v>48</v>
       </c>
-      <c r="J11" s="1">
+      <c r="L16" s="1">
         <v>49</v>
       </c>
-      <c r="K11" s="2">
+      <c r="M16" s="2">
         <v>50</v>
       </c>
-      <c r="L11" s="2">
+      <c r="N16" s="2">
         <v>51</v>
       </c>
-      <c r="M11" s="2">
+      <c r="O16" s="3">
         <v>52</v>
       </c>
-      <c r="N11" s="17"/>
-      <c r="O11" s="18"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="10" t="s">
+    </row>
+    <row r="17" spans="2:19" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="10" t="s">
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="10" t="s">
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+    </row>
+    <row r="18" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="28"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="12"/>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B19" s="28"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="12"/>
+    </row>
+    <row r="20" spans="2:19" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="29"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="16"/>
+    </row>
+    <row r="21" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="N21" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="M12" s="7"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="18"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="18"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="18"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="18"/>
-    </row>
-    <row r="16" spans="1:15" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="16"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="13"/>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="16"/>
+      <c r="O21" s="11"/>
+    </row>
+    <row r="22" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="31"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="12"/>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="31"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="12"/>
+    </row>
+    <row r="24" spans="2:19" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="32"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="16"/>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="O25" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="J10:M10"/>
-    <mergeCell ref="E10:I10"/>
-    <mergeCell ref="D5:D9"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="L12:L16"/>
-    <mergeCell ref="E5:E9"/>
-    <mergeCell ref="K5:K9"/>
-    <mergeCell ref="D12:D16"/>
-    <mergeCell ref="I12:I16"/>
+  <mergeCells count="21">
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="N21:N24"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="N5:N9"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="F17:F20"/>
+    <mergeCell ref="K17:K20"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="K3:O3"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="L15:O15"/>
+    <mergeCell ref="G5:G9"/>
+    <mergeCell ref="I5:I9"/>
+    <mergeCell ref="M10:M14"/>
+    <mergeCell ref="M21:M24"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="G21:G24"/>
+    <mergeCell ref="N10:N14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>